<commit_message>
Added a draft of an invoice generator.
</commit_message>
<xml_diff>
--- a/price_data/data (99).xlsx
+++ b/price_data/data (99).xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="170">
   <si>
     <t>Tidsperiod</t>
   </si>
@@ -306,6 +306,222 @@
   </si>
   <si>
     <t>2022-08-28 23:00</t>
+  </si>
+  <si>
+    <t>2022-08-29 00:00</t>
+  </si>
+  <si>
+    <t>2022-08-29 01:00</t>
+  </si>
+  <si>
+    <t>2022-08-29 02:00</t>
+  </si>
+  <si>
+    <t>2022-08-29 03:00</t>
+  </si>
+  <si>
+    <t>2022-08-29 04:00</t>
+  </si>
+  <si>
+    <t>2022-08-29 05:00</t>
+  </si>
+  <si>
+    <t>2022-08-29 06:00</t>
+  </si>
+  <si>
+    <t>2022-08-29 07:00</t>
+  </si>
+  <si>
+    <t>2022-08-29 08:00</t>
+  </si>
+  <si>
+    <t>2022-08-29 09:00</t>
+  </si>
+  <si>
+    <t>2022-08-29 10:00</t>
+  </si>
+  <si>
+    <t>2022-08-29 11:00</t>
+  </si>
+  <si>
+    <t>2022-08-29 12:00</t>
+  </si>
+  <si>
+    <t>2022-08-29 13:00</t>
+  </si>
+  <si>
+    <t>2022-08-29 14:00</t>
+  </si>
+  <si>
+    <t>2022-08-29 15:00</t>
+  </si>
+  <si>
+    <t>2022-08-29 16:00</t>
+  </si>
+  <si>
+    <t>2022-08-29 17:00</t>
+  </si>
+  <si>
+    <t>2022-08-29 18:00</t>
+  </si>
+  <si>
+    <t>2022-08-29 19:00</t>
+  </si>
+  <si>
+    <t>2022-08-29 20:00</t>
+  </si>
+  <si>
+    <t>2022-08-29 21:00</t>
+  </si>
+  <si>
+    <t>2022-08-29 22:00</t>
+  </si>
+  <si>
+    <t>2022-08-29 23:00</t>
+  </si>
+  <si>
+    <t>2022-08-30 00:00</t>
+  </si>
+  <si>
+    <t>2022-08-30 01:00</t>
+  </si>
+  <si>
+    <t>2022-08-30 02:00</t>
+  </si>
+  <si>
+    <t>2022-08-30 03:00</t>
+  </si>
+  <si>
+    <t>2022-08-30 04:00</t>
+  </si>
+  <si>
+    <t>2022-08-30 05:00</t>
+  </si>
+  <si>
+    <t>2022-08-30 06:00</t>
+  </si>
+  <si>
+    <t>2022-08-30 07:00</t>
+  </si>
+  <si>
+    <t>2022-08-30 08:00</t>
+  </si>
+  <si>
+    <t>2022-08-30 09:00</t>
+  </si>
+  <si>
+    <t>2022-08-30 10:00</t>
+  </si>
+  <si>
+    <t>2022-08-30 11:00</t>
+  </si>
+  <si>
+    <t>2022-08-30 12:00</t>
+  </si>
+  <si>
+    <t>2022-08-30 13:00</t>
+  </si>
+  <si>
+    <t>2022-08-30 14:00</t>
+  </si>
+  <si>
+    <t>2022-08-30 15:00</t>
+  </si>
+  <si>
+    <t>2022-08-30 16:00</t>
+  </si>
+  <si>
+    <t>2022-08-30 17:00</t>
+  </si>
+  <si>
+    <t>2022-08-30 18:00</t>
+  </si>
+  <si>
+    <t>2022-08-30 19:00</t>
+  </si>
+  <si>
+    <t>2022-08-30 20:00</t>
+  </si>
+  <si>
+    <t>2022-08-30 21:00</t>
+  </si>
+  <si>
+    <t>2022-08-30 22:00</t>
+  </si>
+  <si>
+    <t>2022-08-30 23:00</t>
+  </si>
+  <si>
+    <t>2022-08-31 00:00</t>
+  </si>
+  <si>
+    <t>2022-08-31 01:00</t>
+  </si>
+  <si>
+    <t>2022-08-31 02:00</t>
+  </si>
+  <si>
+    <t>2022-08-31 03:00</t>
+  </si>
+  <si>
+    <t>2022-08-31 04:00</t>
+  </si>
+  <si>
+    <t>2022-08-31 05:00</t>
+  </si>
+  <si>
+    <t>2022-08-31 06:00</t>
+  </si>
+  <si>
+    <t>2022-08-31 07:00</t>
+  </si>
+  <si>
+    <t>2022-08-31 08:00</t>
+  </si>
+  <si>
+    <t>2022-08-31 09:00</t>
+  </si>
+  <si>
+    <t>2022-08-31 10:00</t>
+  </si>
+  <si>
+    <t>2022-08-31 11:00</t>
+  </si>
+  <si>
+    <t>2022-08-31 12:00</t>
+  </si>
+  <si>
+    <t>2022-08-31 13:00</t>
+  </si>
+  <si>
+    <t>2022-08-31 14:00</t>
+  </si>
+  <si>
+    <t>2022-08-31 15:00</t>
+  </si>
+  <si>
+    <t>2022-08-31 16:00</t>
+  </si>
+  <si>
+    <t>2022-08-31 17:00</t>
+  </si>
+  <si>
+    <t>2022-08-31 18:00</t>
+  </si>
+  <si>
+    <t>2022-08-31 19:00</t>
+  </si>
+  <si>
+    <t>2022-08-31 20:00</t>
+  </si>
+  <si>
+    <t>2022-08-31 21:00</t>
+  </si>
+  <si>
+    <t>2022-08-31 22:00</t>
+  </si>
+  <si>
+    <t>2022-08-31 23:00</t>
   </si>
 </sst>
 </file>
@@ -350,7 +566,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B98" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B170" headerRowCount="0">
   <tableColumns count="2">
     <tableColumn id="1" name="Tidsperiod"/>
     <tableColumn id="2" name="25 aug 2022 - 31 aug 2022"/>
@@ -361,7 +577,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B97"/>
+  <dimension ref="A1:B169"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -960,7 +1176,7 @@
         <v>74</v>
       </c>
       <c r="B74" s="0">
-        <v>0</v>
+        <v>235.78</v>
       </c>
     </row>
     <row r="75">
@@ -968,7 +1184,7 @@
         <v>75</v>
       </c>
       <c r="B75" s="0">
-        <v>0</v>
+        <v>46.24</v>
       </c>
     </row>
     <row r="76">
@@ -976,7 +1192,7 @@
         <v>76</v>
       </c>
       <c r="B76" s="0">
-        <v>0</v>
+        <v>14.94</v>
       </c>
     </row>
     <row r="77">
@@ -984,7 +1200,7 @@
         <v>77</v>
       </c>
       <c r="B77" s="0">
-        <v>0</v>
+        <v>14.34</v>
       </c>
     </row>
     <row r="78">
@@ -992,7 +1208,7 @@
         <v>78</v>
       </c>
       <c r="B78" s="0">
-        <v>0</v>
+        <v>13.48</v>
       </c>
     </row>
     <row r="79">
@@ -1000,7 +1216,7 @@
         <v>79</v>
       </c>
       <c r="B79" s="0">
-        <v>0</v>
+        <v>12.61</v>
       </c>
     </row>
     <row r="80">
@@ -1008,7 +1224,7 @@
         <v>80</v>
       </c>
       <c r="B80" s="0">
-        <v>0</v>
+        <v>10.56</v>
       </c>
     </row>
     <row r="81">
@@ -1016,7 +1232,7 @@
         <v>81</v>
       </c>
       <c r="B81" s="0">
-        <v>0</v>
+        <v>14.19</v>
       </c>
     </row>
     <row r="82">
@@ -1024,7 +1240,7 @@
         <v>82</v>
       </c>
       <c r="B82" s="0">
-        <v>0</v>
+        <v>15.89</v>
       </c>
     </row>
     <row r="83">
@@ -1032,7 +1248,7 @@
         <v>83</v>
       </c>
       <c r="B83" s="0">
-        <v>0</v>
+        <v>17.46</v>
       </c>
     </row>
     <row r="84">
@@ -1040,7 +1256,7 @@
         <v>84</v>
       </c>
       <c r="B84" s="0">
-        <v>0</v>
+        <v>247.78</v>
       </c>
     </row>
     <row r="85">
@@ -1048,7 +1264,7 @@
         <v>85</v>
       </c>
       <c r="B85" s="0">
-        <v>0</v>
+        <v>266.5</v>
       </c>
     </row>
     <row r="86">
@@ -1056,7 +1272,7 @@
         <v>86</v>
       </c>
       <c r="B86" s="0">
-        <v>0</v>
+        <v>120.33</v>
       </c>
     </row>
     <row r="87">
@@ -1064,7 +1280,7 @@
         <v>87</v>
       </c>
       <c r="B87" s="0">
-        <v>0</v>
+        <v>78.64</v>
       </c>
     </row>
     <row r="88">
@@ -1072,7 +1288,7 @@
         <v>88</v>
       </c>
       <c r="B88" s="0">
-        <v>0</v>
+        <v>13.79</v>
       </c>
     </row>
     <row r="89">
@@ -1080,7 +1296,7 @@
         <v>89</v>
       </c>
       <c r="B89" s="0">
-        <v>0</v>
+        <v>64.49</v>
       </c>
     </row>
     <row r="90">
@@ -1088,7 +1304,7 @@
         <v>90</v>
       </c>
       <c r="B90" s="0">
-        <v>0</v>
+        <v>109.89</v>
       </c>
     </row>
     <row r="91">
@@ -1096,7 +1312,7 @@
         <v>91</v>
       </c>
       <c r="B91" s="0">
-        <v>0</v>
+        <v>255.06</v>
       </c>
     </row>
     <row r="92">
@@ -1104,7 +1320,7 @@
         <v>92</v>
       </c>
       <c r="B92" s="0">
-        <v>0</v>
+        <v>281.79</v>
       </c>
     </row>
     <row r="93">
@@ -1112,7 +1328,7 @@
         <v>93</v>
       </c>
       <c r="B93" s="0">
-        <v>0</v>
+        <v>242.82</v>
       </c>
     </row>
     <row r="94">
@@ -1120,7 +1336,7 @@
         <v>94</v>
       </c>
       <c r="B94" s="0">
-        <v>0</v>
+        <v>255.11</v>
       </c>
     </row>
     <row r="95">
@@ -1128,7 +1344,7 @@
         <v>95</v>
       </c>
       <c r="B95" s="0">
-        <v>0</v>
+        <v>253.58</v>
       </c>
     </row>
     <row r="96">
@@ -1136,7 +1352,7 @@
         <v>96</v>
       </c>
       <c r="B96" s="0">
-        <v>0</v>
+        <v>10.34</v>
       </c>
     </row>
     <row r="97">
@@ -1144,7 +1360,583 @@
         <v>97</v>
       </c>
       <c r="B97" s="0">
-        <v>0</v>
+        <v>8.91</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B98" s="0">
+        <v>8.8</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B99" s="0">
+        <v>8.16</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="B100" s="0">
+        <v>7.39</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="B101" s="0">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="B102" s="0">
+        <v>10.62</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B103" s="0">
+        <v>14.4</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B104" s="0">
+        <v>19.11</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B105" s="0">
+        <v>415.76</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B106" s="0">
+        <v>595.24</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B107" s="0">
+        <v>563.36</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="B108" s="0">
+        <v>563.34</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="B109" s="0">
+        <v>595.77</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="B110" s="0">
+        <v>530.49</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B111" s="0">
+        <v>496.12</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="B112" s="0">
+        <v>512.04</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B113" s="0">
+        <v>478.28</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="B114" s="0">
+        <v>426.34</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B115" s="0">
+        <v>478.29</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="B116" s="0">
+        <v>513.75</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B117" s="0">
+        <v>468.98</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B118" s="0">
+        <v>416.92</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B119" s="0">
+        <v>318.88</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B120" s="0">
+        <v>154.12</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B121" s="0">
+        <v>19.87</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="B122" s="0">
+        <v>22.37</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B123" s="0">
+        <v>20.91</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B124" s="0">
+        <v>21.36</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="B125" s="0">
+        <v>21.72</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B126" s="0">
+        <v>26.67</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B127" s="0">
+        <v>59.8</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="B128" s="0">
+        <v>324.97</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="B129" s="0">
+        <v>808.13</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="B130" s="0">
+        <v>821.89</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="B131" s="0">
+        <v>789.33</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="B132" s="0">
+        <v>707.47</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B133" s="0">
+        <v>617.51</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="B134" s="0">
+        <v>605.89</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B135" s="0">
+        <v>608.67</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="B136" s="0">
+        <v>589.54</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="B137" s="0">
+        <v>618.62</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="B138" s="0">
+        <v>610.73</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B139" s="0">
+        <v>739.56</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B140" s="0">
+        <v>824.39</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B141" s="0">
+        <v>851.33</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="B142" s="0">
+        <v>786.97</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="B143" s="0">
+        <v>603.96</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B144" s="0">
+        <v>362.64</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B145" s="0">
+        <v>210.19</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B146" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B147" s="0">
+        <v>26.1</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="B148" s="0">
+        <v>24.99</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B149" s="0">
+        <v>24.35</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B150" s="0">
+        <v>24.72</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B151" s="0">
+        <v>143.64</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B152" s="0">
+        <v>295.44</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B153" s="0">
+        <v>660.69</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B154" s="0">
+        <v>749.92</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="B155" s="0">
+        <v>686.11</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="B156" s="0">
+        <v>674.87</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="B157" s="0">
+        <v>687.15</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B158" s="0">
+        <v>589.22</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="B159" s="0">
+        <v>563.8</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="B160" s="0">
+        <v>529.59</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="B161" s="0">
+        <v>479.51</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="B162" s="0">
+        <v>499.42</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="B163" s="0">
+        <v>639.31</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="B164" s="0">
+        <v>660.6</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="B165" s="0">
+        <v>639.36</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="B166" s="0">
+        <v>635.3</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="B167" s="0">
+        <v>470.94</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="B168" s="0">
+        <v>207.81</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="B169" s="0">
+        <v>26.58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>